<commit_message>
1/11 end of day
</commit_message>
<xml_diff>
--- a/project_details/capstone roadmap.xlsx
+++ b/project_details/capstone roadmap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11900" yWindow="320" windowWidth="29520" windowHeight="19780" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="880" yWindow="0" windowWidth="25600" windowHeight="13200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Roadmap" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Goal</t>
   </si>
@@ -119,6 +119,23 @@
   </si>
   <si>
     <t>NMF</t>
+  </si>
+  <si>
+    <t>presentation / insights / slides</t>
+  </si>
+  <si>
+    <t>presentation / slides</t>
+  </si>
+  <si>
+    <t>modeling
+user testing</t>
+  </si>
+  <si>
+    <t>Word2vec model
+NMF Model</t>
+  </si>
+  <si>
+    <t>Ensemble Model</t>
   </si>
 </sst>
 </file>
@@ -281,6 +298,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -298,9 +318,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -639,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -658,13 +675,13 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="3">
@@ -730,13 +747,13 @@
       <c r="F9" s="2"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" s="3">
@@ -759,11 +776,21 @@
       <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="B13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="59" customHeight="1">
       <c r="A14" s="4" t="s">
@@ -788,12 +815,12 @@
       <c r="F15" s="2"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="3">
@@ -817,7 +844,7 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -828,7 +855,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="9"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:6" ht="43" customHeight="1">
       <c r="A21" s="4" t="s">
@@ -837,7 +864,7 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="9"/>
+      <c r="E21" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -860,7 +887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -889,7 +916,7 @@
       <c r="B2" s="8">
         <v>42374</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="9" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>